<commit_message>
3rd Functionality is reworked and now working
</commit_message>
<xml_diff>
--- a/Information of MTR lines.xlsx
+++ b/Information of MTR lines.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KKGM013/Documents/Aston Stuff/Year 2/CS2310/Coursework/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KKGM013/Documents/Aston Stuff/Year 2/CS2310/Coursework/MTRCS2310/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="109">
   <si>
     <t>Airport Express</t>
   </si>
@@ -339,6 +339,21 @@
   </si>
   <si>
     <t>Associated Lines</t>
+  </si>
+  <si>
+    <t>Tung Chung Line &amp; Walkable</t>
+  </si>
+  <si>
+    <t>Walkable, Tsuen Wan Line, South Island Line &amp; Tseung Kwan O Line</t>
+  </si>
+  <si>
+    <t>Kwun Tong Line, Ma On Shan Line &amp; West Rail Line</t>
+  </si>
+  <si>
+    <t>Tsuen Wan Line, Tseung Kwan O Line &amp; East Rail Line</t>
+  </si>
+  <si>
+    <t>Tsuen Wan Line &amp; Island Line</t>
   </si>
 </sst>
 </file>
@@ -485,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -493,7 +508,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -506,11 +520,17 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,8 +819,8 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B13" sqref="B13"/>
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -829,46 +849,46 @@
       <c r="A1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
       <c r="S1" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="4"/>
@@ -883,21 +903,26 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
-      <c r="S2" s="5"/>
+      <c r="S2" s="19" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
+      <c r="S3" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
@@ -924,21 +949,24 @@
       <c r="I4" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="8" t="s">
         <v>19</v>
       </c>
       <c r="L4" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="8" t="s">
         <v>21</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B5" t="s">
@@ -953,10 +981,10 @@
       <c r="E5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>28</v>
       </c>
       <c r="H5" t="s">
@@ -971,10 +999,10 @@
       <c r="K5" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="9" t="s">
         <v>34</v>
       </c>
       <c r="N5" t="s">
@@ -992,9 +1020,12 @@
       <c r="R5" t="s">
         <v>39</v>
       </c>
+      <c r="S5" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>40</v>
       </c>
       <c r="B6" t="s">
@@ -1003,19 +1034,19 @@
       <c r="C6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G6" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I6" t="s">
@@ -1042,18 +1073,21 @@
       <c r="P6" t="s">
         <v>54</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="Q6" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="R6" s="10" t="s">
         <v>56</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C7" t="s">
@@ -1080,9 +1114,12 @@
       <c r="J7" t="s">
         <v>65</v>
       </c>
+      <c r="S7" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>66</v>
       </c>
       <c r="B8" t="s">
@@ -1097,24 +1134,27 @@
       <c r="E8" t="s">
         <v>70</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>28</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>56</v>
       </c>
       <c r="F9" t="s">
@@ -1128,7 +1168,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="21" t="s">
         <v>75</v>
       </c>
       <c r="B10" t="s">
@@ -1143,10 +1183,10 @@
       <c r="E10" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>81</v>
       </c>
       <c r="H10" t="s">
@@ -1158,13 +1198,13 @@
       <c r="J10" t="s">
         <v>84</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="L10" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="M10" s="10" t="s">
         <v>43</v>
       </c>
       <c r="N10" t="s">
@@ -1173,35 +1213,35 @@
       <c r="O10" t="s">
         <v>86</v>
       </c>
-      <c r="P10" s="10" t="s">
+      <c r="P10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="Q10" s="10" t="s">
+      <c r="Q10" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>87</v>
       </c>
       <c r="B11" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>89</v>
       </c>
       <c r="B12" t="s">
@@ -1225,7 +1265,7 @@
       <c r="H12" t="s">
         <v>96</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="I12" s="15" t="s">
         <v>81</v>
       </c>
       <c r="J12" t="s">
@@ -1237,18 +1277,18 @@
       <c r="L12" t="s">
         <v>99</v>
       </c>
-      <c r="M12" s="9" t="s">
+      <c r="M12" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes and having the last get the user data
</commit_message>
<xml_diff>
--- a/Information of MTR lines.xlsx
+++ b/Information of MTR lines.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="114">
   <si>
     <t>Airport Express</t>
   </si>
@@ -354,6 +354,21 @@
   </si>
   <si>
     <t>Tsuen Wan Line &amp; Island Line</t>
+  </si>
+  <si>
+    <t>Island Line &amp; Kwun Tong Line</t>
+  </si>
+  <si>
+    <t>South Island Line, Island Line, Walkable, Kwun Tong Line &amp; West Rail Line</t>
+  </si>
+  <si>
+    <t>Airport Express, Walkable &amp; Disneyland Resort Line</t>
+  </si>
+  <si>
+    <t>Tsuen Wan Line &amp; East Rail Line</t>
+  </si>
+  <si>
+    <t>Airport Express, Tsuen Wan Line, Island Line &amp; Tung Chung Line</t>
   </si>
 </sst>
 </file>
@@ -819,8 +834,8 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S8" sqref="S8"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1166,6 +1181,9 @@
       <c r="H9" t="s">
         <v>74</v>
       </c>
+      <c r="S9" s="2" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
@@ -1219,6 +1237,9 @@
       <c r="Q10" s="9" t="s">
         <v>27</v>
       </c>
+      <c r="S10" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
@@ -1239,6 +1260,9 @@
       <c r="F11" s="17" t="s">
         <v>5</v>
       </c>
+      <c r="S11" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
@@ -1280,6 +1304,9 @@
       <c r="M12" s="8" t="s">
         <v>21</v>
       </c>
+      <c r="S12" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
@@ -1290,6 +1317,9 @@
       </c>
       <c r="C13" s="9" t="s">
         <v>27</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>